<commit_message>
Interpret xlsx comments with no text correctly
</commit_message>
<xml_diff>
--- a/tests/test_comments_excel.xlsx
+++ b/tests/test_comments_excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -96,9 +97,22 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text/>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +129,13 @@
     <font>
       <b/>
       <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
@@ -231,7 +252,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -266,7 +286,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,16 +461,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -460,16 +477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -478,18 +493,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="597" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>